<commit_message>
feat: improve questionnaire mode
</commit_message>
<xml_diff>
--- a/tools/sample/questionnaire.xlsx
+++ b/tools/sample/questionnaire.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
   <si>
     <t xml:space="preserve">library_urn</t>
   </si>
@@ -96,12 +96,6 @@
     <t xml:space="preserve">framework_description</t>
   </si>
   <si>
-    <t xml:space="preserve">framework_min_score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">framework_max_score</t>
-  </si>
-  <si>
     <t xml:space="preserve">tab</t>
   </si>
   <si>
@@ -147,7 +141,7 @@
     <t xml:space="preserve">Q1</t>
   </si>
   <si>
-    <t xml:space="preserve">Niveau de criticité des projets</t>
+    <t xml:space="preserve">Niveau de criticité du projet</t>
   </si>
   <si>
     <t xml:space="preserve">1 - Faible
@@ -160,6 +154,67 @@
   </si>
   <si>
     <t xml:space="preserve">A2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durée du projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 – Quelques semaines
+2 – Quelques mois
+3 – Quelques années
+4 – Une dizaine d’années</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quelle est la durée du projet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exposition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le projet sera-t-il exposé sur le web ?
+Le projet sera-t-il sur instance On-prem ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les données du projet sont-elles confidentielles ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Démarrage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quand le projet démarrera-t-il ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qui sera responsable du projet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5</t>
   </si>
   <si>
     <t xml:space="preserve">MATURITY</t>
@@ -324,6 +379,17 @@
 2
 3
 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes
+No
+N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
   </si>
 </sst>
 </file>
@@ -443,10 +509,10 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.25"/>
@@ -557,44 +623,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1" t="n">
-        <v>0</v>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
+      <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -612,43 +664,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,244 +708,347 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="0" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="G4" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="0" t="s">
         <v>53</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="0" t="s">
         <v>56</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="0" t="s">
         <v>59</v>
       </c>
+      <c r="F8" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="G8" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="166.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>50</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="166.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -912,48 +1067,75 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>83</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add question update
</commit_message>
<xml_diff>
--- a/tools/sample/questionnaire.xlsx
+++ b/tools/sample/questionnaire.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="112">
   <si>
     <t xml:space="preserve">library_urn</t>
   </si>
@@ -144,12 +144,6 @@
     <t xml:space="preserve">Niveau de criticité du projet</t>
   </si>
   <si>
-    <t xml:space="preserve">1 - Faible
-2 - Modérée
-3 - Forte
-4 - Critique</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quel est le niveau de criticité du projet métier ?</t>
   </si>
   <si>
@@ -162,13 +156,10 @@
     <t xml:space="preserve">Durée du projet</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – Quelques semaines
-2 – Quelques mois
-3 – Quelques années
-4 – Une dizaine d’années</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quelle est la durée du projet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6</t>
   </si>
   <si>
     <t xml:space="preserve">Q3</t>
@@ -227,6 +218,102 @@
   </si>
   <si>
     <t xml:space="preserve">A.1 - Politique de sécurité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.2 - Formation à la cybersécurité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.3 - Procédures de gestion des incidents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.4 - Surveillance des systèmes d'information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.5 - Plan de continuité des activités (PCA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.6 - Évaluation des risques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.7 - Gestion des sauvegardes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.8 - Protection des données personnelles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.9 - Audit de sécurité interne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.10 - Utilisation des pare-feu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">question_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">question_choices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique_choice</t>
   </si>
   <si>
     <t xml:space="preserve">0 : Aucune politique de sécurité mise en place.
@@ -236,13 +323,27 @@
 4 : La politique de sécurité est pleinement optimisée et améliorée en continu.</t>
   </si>
   <si>
-    <t xml:space="preserve">A1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.2 - Formation à la cybersécurité</t>
+    <t xml:space="preserve">1 - Faible
+2 - Modérée
+3 - Forte
+4 - Critique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes
+No
+N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 – Quelques semaines
+2 – Quelques mois
+3 – Quelques années
+4 – Une dizaine d’années</t>
   </si>
   <si>
     <t xml:space="preserve">0 : Aucune formation à la cybersécurité n'est prévue.
@@ -252,12 +353,6 @@
 4 : Une formation régulière et optimisée est en place, avec suivi et amélioration continue.</t>
   </si>
   <si>
-    <t xml:space="preserve">M3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.3 - Procédures de gestion des incidents</t>
-  </si>
-  <si>
     <t xml:space="preserve">0 : Aucune procédure de gestion des incidents n'est en place.
 1 : Des procédures existent mais ne sont pas formalisées.
 2 : Les procédures sont formalisées mais non encore testées.
@@ -265,12 +360,6 @@
 4 : Les procédures sont optimisées, testées régulièrement et améliorées en continu.</t>
   </si>
   <si>
-    <t xml:space="preserve">M4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.4 - Surveillance des systèmes d'information</t>
-  </si>
-  <si>
     <t xml:space="preserve">0 : Aucune surveillance des systèmes d'information n'est mise en place.
 1 : Une surveillance limitée est mise en place sans automatisation.
 2 : Une surveillance est formalisée mais encore partiellement automatisée.
@@ -278,12 +367,6 @@
 4 : La surveillance est pleinement automatisée et optimisée, avec une réponse rapide aux incidents.</t>
   </si>
   <si>
-    <t xml:space="preserve">M5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.5 - Plan de continuité des activités (PCA)</t>
-  </si>
-  <si>
     <t xml:space="preserve">0 : Aucun plan de continuité des activités n'existe.
 1 : Un PCA est défini mais partiel.
 2 : Le PCA est formalisé mais non encore testé.
@@ -291,12 +374,6 @@
 4 : Le PCA est testé, optimisé et régulièrement mis à jour.</t>
   </si>
   <si>
-    <t xml:space="preserve">M6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.6 - Évaluation des risques</t>
-  </si>
-  <si>
     <t xml:space="preserve">0 : Aucune évaluation des risques n'est réalisée.
 1 : Une évaluation est réalisée de manière informelle.
 2 : Une évaluation formelle des risques est définie mais pas encore réalisée régulièrement.
@@ -304,12 +381,6 @@
 4 : L'évaluation des risques est systématique, optimisée et inclut des actions correctives continues.</t>
   </si>
   <si>
-    <t xml:space="preserve">M7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.7 - Gestion des sauvegardes</t>
-  </si>
-  <si>
     <t xml:space="preserve">0 : Aucune gestion des sauvegardes n'est mise en place.
 1 : Des sauvegardes sont effectuées mais sans formalisation ni test.
 2 : Les sauvegardes sont formalisées mais rarement testées.
@@ -317,12 +388,6 @@
 4 : Les sauvegardes sont optimisées, testées régulièrement, avec restauration rapide garantie.</t>
   </si>
   <si>
-    <t xml:space="preserve">M8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.8 - Protection des données personnelles</t>
-  </si>
-  <si>
     <t xml:space="preserve">0 : Aucune mesure de protection des données personnelles n'est mise en place.
 1 : Quelques mesures de protection sont définies mais insuffisantes.
 2 : Des mesures de protection formalisées sont en place mais non optimisées.
@@ -330,12 +395,6 @@
 4 : Les données personnelles sont pleinement protégées, avec surveillance et optimisation continues.</t>
   </si>
   <si>
-    <t xml:space="preserve">M9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.9 - Audit de sécurité interne</t>
-  </si>
-  <si>
     <t xml:space="preserve">0 : Aucun audit de sécurité interne n'est réalisé.
 1 : Des audits sont réalisés de manière informelle et sporadique.
 2 : Les audits sont formalisés mais réalisés de manière irrégulière.
@@ -343,53 +402,11 @@
 4 : Les audits sont optimisés, réalisés régulièrement, et des améliorations continues sont appliquées.</t>
   </si>
   <si>
-    <t xml:space="preserve">M10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.10 - Utilisation des pare-feu</t>
-  </si>
-  <si>
     <t xml:space="preserve">0 : Aucun pare-feu n'est utilisé.
 1 : Des pare-feu sont déployés mais sans politique de gestion.
 2 : Les pare-feu sont formalisés avec des règles mais non optimisées.
 3 : Les pare-feu sont correctement configurés mais pas encore optimisés.
 4 : Les pare-feu sont pleinement optimisés, avec une gestion et une mise à jour continue des règles.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">question_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">question_choices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unique_choice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0
-1
-2
-3
-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1
-2
-3
-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes
-No
-N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
   </si>
 </sst>
 </file>
@@ -481,11 +498,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -666,8 +683,8 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -714,7 +731,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -727,37 +744,31 @@
       <c r="D3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,16 +779,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="F5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,16 +799,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="G6" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -808,16 +819,16 @@
         <v>2</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -828,16 +839,16 @@
         <v>2</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,30 +856,27 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="G10" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -879,16 +887,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -899,156 +904,132 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="1" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="G13" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="1" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="G14" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="1" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="166.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="G15" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="1" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="G16" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="1" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="G17" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="1" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="G18" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="1" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="G19" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1067,10 +1048,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1080,62 +1061,172 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="280.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C2" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="0" t="s">
+    <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="305.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="344" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="382.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="382.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="382.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="369.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="331.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="318.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>